<commit_message>
Commit file Api design when fix conflict
</commit_message>
<xml_diff>
--- a/doc/API_Design/API_Detail/BLOG_API_SD.xlsx
+++ b/doc/API_Design/API_Detail/BLOG_API_SD.xlsx
@@ -9,11 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Register user" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
+    <sheet name="Logout" sheetId="3" r:id="rId3"/>
+    <sheet name="Update user" sheetId="4" r:id="rId4"/>
+    <sheet name="Get user info" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,12 +28,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>REGISTER USER SEQUENCE DIAGRAM</t>
   </si>
   <si>
     <t>LOGIN SEQUENCE DIAGRAM</t>
+  </si>
+  <si>
+    <t>LOGOUT SEQUENCE DIAGRAM</t>
+  </si>
+  <si>
+    <t>UPDATE USER SEQUENCE DIAGRAM</t>
+  </si>
+  <si>
+    <t>GET USER INFORMATIONS SEQUENCE DIAGRAM</t>
   </si>
 </sst>
 </file>
@@ -230,18 +242,56 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>123826</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
+    <xdr:ext cx="10497964" cy="10039350"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="123826" y="523875"/>
+          <a:ext cx="10497964" cy="10039350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>258590</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>404586</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -258,8 +308,94 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="123826" y="533400"/>
-          <a:ext cx="10497964" cy="10039350"/>
+          <a:off x="485775" y="400050"/>
+          <a:ext cx="9062811" cy="5048250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>370617</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="485775"/>
+          <a:ext cx="10733817" cy="10010775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>99400</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="466725"/>
+          <a:ext cx="9243400" cy="4981575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -537,7 +673,7 @@
   <dimension ref="A1:R53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:M3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1617,8 +1753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView showGridLines="0" topLeftCell="F1" workbookViewId="0">
+      <selection sqref="A1:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1662,4 +1798,157 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:M2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:M2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:M2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:M2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>